<commit_message>
2_5 fixes to model and start of econ framework
</commit_message>
<xml_diff>
--- a/Model 1_29/pneumonia output.xlsx
+++ b/Model 1_29/pneumonia output.xlsx
@@ -157,40 +157,40 @@
     <t>{2014., 0.0879139689742313}</t>
   </si>
   <si>
-    <t>{{2000., 0.13853578631707641}, {2001., 0.14334870031974473}, {2002., 0.15343933769177553}, {2003., 0.16117925782508266}, {2004., 0.1670202902235085}, {2005., 0.17374020273849802}, {2006., 0.17501863662285133}, {2007., 0.1734417474242709}, {2008., 0.17756304988979338}, {2009., 0.17753535724882602}, {2010., 0.17970141043615664}, {2011., 0.19351556568143577}, {2012., 0.20034842357482952}, {2013., 0.1939792989142101}, {2014., 0.1910049071412821}, {2015., 0.20213863177780472}, {2016., 0.21418722433649331}, {2017., 0.21959080139163567}, {2018., 0.2250916524897339}, {2019., 0.2306895689993882}, {2020., 0.2363842349042214}, {2021., 0.24217522357498608}, {2022., 0.24806199470930604}, {2023., 0.2540438914589147}, {2024., 0.26012013776437715}, {2025., 0.2662898359172398}, {2026., 0.27255196436942764}, {2027., 0.2789053758094195}, {2028., 0.2853487955242641}, {2029., 0.29188082006592736}, {2030., 0.29849991623970995}, {2031., 0.30520442043152923}, {2032., 0.31199253828980067}, {2033., 0.3188623447764204}, {2034., 0.3258117845999054}, {2035., 0.33283867304222275}, {2036., 0.3399406971891199}, {2037., 0.347115417571885}, {2038., 0.3543602702264999}, {2039., 0.3616725691740388}, {2040., 0.3690495093239103}}</t>
-  </si>
-  <si>
-    <t>{{2000., 0.17779003343384756}, {2001., 0.1848369219848541}, {2002., 0.19965519201795298}, {2003., 0.21104186375044948}, {2004., 0.2196410674418312}, {2005., 0.22953585759734904}, {2006., 0.2314181267257109}, {2007., 0.22909641892407562}, {2008., 0.23516390241792803}, {2009., 0.23512313821348926}, {2010., 0.23831131833515012}, {2011., 0.2586215375621919}, {2012., 0.26864583836891837}, {2013., 0.25930241337483295}, {2014., 0.2549340343450744}, {2015., 0.27126909467423665}, {2016., 0.2888839482126477}, {2017., 0.29675767464418734}, {2018., 0.30475403478292823}, {2019., 0.3128700019636655}, {2020., 0.3211022828894477}, {2021., 0.32944731871954214}, {2022., 0.3379012873082604}, {2023., 0.34646010662732046}, {2024., 0.3551194393965171}, {2025., 0.3638746989388802}, {2026., 0.37272105626741503}, {2027., 0.3816534484009242}, {2028., 0.3906665878963967}, {2029., 0.39975497357525136}, {2030., 0.4089129024103452}, {2031., 0.4181344825302261}, {2032., 0.42741364728688075}, {2033., 0.4367441703232275}, {2034., 0.4461196815669581}, {2035., 0.4555336840683105}, {2036., 0.46497957159096026}, {2037., 0.4744506468575914}, {2038., 0.48394014034505733}, {2039., 0.49344122951839203}, {2040., 0.5029470583883212}}</t>
-  </si>
-  <si>
-    <t>{{2000., 0.0626042080198429}, {2001., 0.07828185182181285}, {2002., 0.12099826774212379}, {2003., 0.16366198507770507}, {2004., 0.20049854347802348}, {2005., 0.2473145590665686}, {2006., 0.25470643379996355}, {2007., 0.23999846173497844}, {2008., 0.268978845725233}, {2009., 0.26588817556872296}, {2010., 0.27971215798178056}, {2011., 0.3932230520697693}, {2012., 0.45209508286717653}, {2013., 0.3952393306704061}, {2014., 0.36907072171796856}, {2015., 0.46812176495997004}, {2016., 0.5734396625600047}, {2017., 0.6178007346694113}, {2018., 0.6602814776922612}, {2019., 0.7003308414017303}, {2020., 0.7375355717946492}, {2021., 0.7716274774572838}, {2022., 0.8024770840558872}, {2023., 0.8300770822479615}, {2024., 0.8545196688213008}, {2025., 0.8759716533661583}, {2026., 0.8946503879394989}, {2027., 0.9108025370128678}, {2028., 0.9246867179085829}, {2029., 0.93656026403774}, {2030., 0.9466698425854797}, {2031., 0.9552453721750656}, {2032., 0.9624965788944643}, {2033., 0.9686115395479054}, {2034., 0.9737566367907494}, {2035., 0.9780774538691314}, {2036., 0.9817002428062278}, {2037., 0.9847336957907679}, {2038., 0.9872708295224226}, {2039., 0.98939085527607}, {2040., 0.9911609548644303}}</t>
-  </si>
-  <si>
-    <t>{{2000., 0.11341260818775203}, {2001., 0.14596871370570527}, {2002., 0.23426866295908763}, {2003., 0.31892802251995606}, {2004., 0.38792268641414973}, {2005., 0.46844681062458376}, {2006., 0.4804086349471679}, {2007., 0.4564055669953613}, {2008., 0.5029272342798269}, {2009., 0.4981151391638927}, {2010., 0.5193648131117024}, {2011., 0.6687211359701506}, {2012., 0.7305533231766058}, {2013., 0.671001375145701}, {2014., 0.6404607203482999}, {2015., 0.7457800707439324}, {2016., 0.8311131594199891}, {2017., 0.8604034764358723}, {2018., 0.8853148961587166}, {2019., 0.9062651058965333}, {2020., 0.9237179733953593}, {2021., 0.9381430251838081}, {2022., 0.949987965716772}, {2023., 0.9596622542947404}, {2024., 0.9675291206713849}, {2025., 0.9739034730618871}, {2026., 0.9790535684397658}, {2027., 0.9832048305456308}, {2028., 0.9865446827948882}, {2029., 0.9892276557467177}, {2030., 0.9913803216022361}, {2031., 0.9931058125716821}, {2032., 0.9944878145242669}, {2033., 0.9955940108260402}, {2034., 0.9964789994346714}, {2035., 0.9971867312026996}, {2036., 0.9977525275904343}, {2037., 0.9982047375260265}, {2038., 0.9985660898658996}, {2039., 0.998854792267173}, {2040., 0.9990854207796269}}</t>
-  </si>
-  <si>
-    <t>{{2000., 0.004245667881577086}, {2001., 0.004874671535597712}, {2002., 0.006432322750266142}, {2003., 0.007875456858226432}, {2004., 0.009763968474068623}, {2005., 0.013322623847923817}, {2006., 0.015878728835289017}, {2007., 0.01763802116239439}, {2008., 0.023309190697007875}, {2009., 0.027144017106482086}, {2010., 0.034581371851898364}, {2011., 0.06473052508448475}, {2012., 0.08767532860592818}, {2013., 0.07171296748522162}, {2014., 0.06510170723603599}, {2015., 0.0926303218972931}, {2016., 0.13178452070449528}, {2017., 0.15281867943768995}, {2018., 0.17652749826032493}, {2019., 0.20303306200913526}, {2020., 0.23239527455789497}, {2021., 0.26459401101631946}, {2022., 0.2995132146566304}, {2023., 0.3369294510829289}, {2024., 0.37650751724916703}, {2025., 0.4178052589725179}, {2026., 0.46028870918871795}, {2027., 0.5033571257206966}, {2028., 0.5463757808166617}, {2029., 0.5887128645646381}, {2030., 0.629776030765698}, {2031., 0.669044187389696}, {2032., 0.7060910918557864}, {2033., 0.7405988680993955}, {2034., 0.7723612851039866}, {2035., 0.801278108512984}, {2036., 0.8273427873082795}, {2037., 0.8506260911239745}, {2038., 0.8712581602717802}, {2039., 0.8894109493943749}, {2040., 0.9052824284544828}}</t>
-  </si>
-  <si>
-    <t>{{2000., 0.0066921836593021936}, {2001., 0.007910345154487044}, {2002., 0.011061368771239552}, {2003., 0.014123144211918903}, {2004., 0.018321636382292398}, {2005., 0.026659366655086326}, {2006., 0.03291801690740733}, {2007., 0.03733171127755734}, {2008., 0.05202414690300587}, {2009., 0.06227050526078328}, {2010., 0.08263074785857878}, {2011., 0.1674998458143094}, {2012., 0.23095523189373252}, {2013., 0.18704726231150867}, {2014., 0.16854286173802427}, {2015., 0.2443090418834672}, {2016., 0.3440736651995076}, {2017., 0.39303430700301767}, {2018., 0.44424334921232117}, {2019., 0.4966648793326893}, {2020., 0.5491598351588212}, {2021., 0.6005827937086953}, {2022., 0.6498799026176181}, {2023., 0.6961706650246423}, {2024., 0.7388010006574828}, {2025., 0.7773627576095049}, {2026., 0.8116826280037501}, {2027., 0.8417887686178006}, {2028., 0.8678653858244724}, {2029., 0.8902046061727308}, {2030., 0.9091623717024868}, {2031., 0.9251221345050487}, {2032., 0.9384676182760775}, {2033., 0.9495642107589123}, {2034., 0.9587476361347855}, {2035., 0.9663182412079145}, {2036., 0.9725392883173026}, {2037., 0.9776378935679481}, {2038., 0.9818075536608285}, {2039., 0.9852114956261768}, {2040., 0.9879863280640039}}</t>
-  </si>
-  <si>
-    <t>{{2014., 0.1910049071412821}, {2015., 0.19306964114232217}, {2016., 0.19306964114232217}, {2017., 0.19306964114232217}, {2018., 0.18799165983141938}, {2019., 0.178144990914702}, {2020., 0.1687069179974608}, {2021., 0.15967172539517838}, {2022., 0.15103250351512018}, {2023., 0.1427812941418837}, {2024., 0.1387984553078299}, {2025., 0.1387984553078299}, {2026., 0.1387984553078299}, {2027., 0.1387984553078299}, {2028., 0.1387984553078299}, {2029., 0.1387984553078299}, {2030., 0.1387984553078299}, {2031., 0.1387984553078299}, {2032., 0.1387984553078299}, {2033., 0.1387984553078299}, {2034., 0.1387984553078299}, {2035., 0.1387984553078299}, {2036., 0.1387984553078299}, {2037., 0.1387984553078299}, {2038., 0.1387984553078299}, {2039., 0.1387984553078299}, {2040., 0.1387984553078299}}</t>
-  </si>
-  <si>
-    <t>{{2014., 0.2549340343450744}, {2015., 0.2579667406511518}, {2016., 0.2579667406511518}, {2017., 0.2579667406511518}, {2018., 0.25050583030341017}, {2019., 0.23602051136483967}, {2020., 0.22212455849339827}, {2021., 0.20882311751577545}, {2022., 0.19611738415388097}, {2023., 0.1840049298409873}, {2024., 0.1781737503104796}, {2025., 0.1781737503104796}, {2026., 0.1781737503104796}, {2027., 0.1781737503104796}, {2028., 0.1781737503104796}, {2029., 0.1781737503104796}, {2030., 0.1781737503104796}, {2031., 0.1781737503104796}, {2032., 0.1781737503104796}, {2033., 0.1781737503104796}, {2034., 0.1781737503104796}, {2035., 0.1781737503104796}, {2036., 0.1781737503104796}, {2037., 0.1781737503104796}, {2038., 0.1781737503104796}, {2039., 0.1781737503104796}, {2040., 0.1781737503104796}}</t>
-  </si>
-  <si>
-    <t>{{2014., 0.36907072171796856}, {2015., 0.3871972894201271}, {2016., 0.3871972894201271}, {2017., 0.3871972894201271}, {2018., 0.343018602053508}, {2019., 0.2628136076010174}, {2020., 0.19577384440165335}, {2021., 0.14244522970796508}, {2022., 0.10144779782988142}, {2023., 0.07126928294352983}, {2024., 0.05950142355913755}, {2025., 0.05950142355913755}, {2026., 0.05950142355913755}, {2027., 0.05950142355913755}, {2028., 0.05950142355913755}, {2029., 0.05950142355913755}, {2030., 0.05950142355913755}, {2031., 0.05950142355913755}, {2032., 0.05950142355913755}, {2033., 0.05950142355913755}, {2034., 0.05950142355913755}, {2035., 0.05950142355913755}, {2036., 0.05950142355913755}, {2037., 0.05950142355913755}, {2038., 0.05950142355913755}, {2039., 0.05950142355913755}, {2040., 0.05950142355913755}}</t>
-  </si>
-  <si>
-    <t>{{2014., 0.6404607203482999}, {2015., 0.6618342484560983}, {2016., 0.6618342484560983}, {2017., 0.6618342484560983}, {2018., 0.6079440132351323}, {2019., 0.49329293632400073}, {2020., 0.3793429802436148}, {2021., 0.2773096938948378}, {2022., 0.19413633941442557}, {2023., 0.13137429103220008}, {2024., 0.10701355548726615}, {2025., 0.10701355548726615}, {2026., 0.10701355548726615}, {2027., 0.10701355548726615}, {2028., 0.10701355548726615}, {2029., 0.10701355548726615}, {2030., 0.10701355548726615}, {2031., 0.10701355548726615}, {2032., 0.10701355548726615}, {2033., 0.10701355548726615}, {2034., 0.10701355548726615}, {2035., 0.10701355548726615}, {2036., 0.10701355548726615}, {2037., 0.10701355548726615}, {2038., 0.10701355548726615}, {2039., 0.10701355548726615}, {2040., 0.10701355548726615}}</t>
-  </si>
-  <si>
-    <t>{{2014., 0.06510170723603599}, {2015., 0.06963624210755885}, {2016., 0.06963624210755885}, {2017., 0.06963624210755885}, {2018., 0.05891554894453729}, {2019., 0.041958803172235035}, {2020., 0.02972828495333086}, {2021., 0.020984736649181754}, {2022., 0.01477364496720295}, {2023., 0.010381426927592325}, {2024., 0.008697892419487157}, {2025., 0.008697892419487157}, {2026., 0.008697892419487157}, {2027., 0.008697892419487157}, {2028., 0.008697892419487157}, {2029., 0.008697892419487157}, {2030., 0.008697892419487157}, {2031., 0.008697892419487157}, {2032., 0.008697892419487157}, {2033., 0.008697892419487157}, {2034., 0.008697892419487157}, {2035., 0.008697892419487157}, {2036., 0.008697892419487157}, {2037., 0.008697892419487157}, {2038., 0.008697892419487157}, {2039., 0.008697892419487157}, {2040., 0.008697892419487157}}</t>
-  </si>
-  <si>
-    <t>{{2014., 0.16854286173802427}, {2015., 0.1812508665621468}, {2016., 0.1812508665621468}, {2017., 0.1812508665621468}, {2018., 0.15111679357710947}, {2019., 0.10323235151916754}, {2020., 0.0692826955379296}, {2021., 0.045926154014675695}, {2022., 0.030188161731358028}, {2023., 0.019731733017928087}, {2024., 0.015928774696171277}, {2025., 0.015928774696171277}, {2026., 0.015928774696171277}, {2027., 0.015928774696171277}, {2028., 0.015928774696171277}, {2029., 0.015928774696171277}, {2030., 0.015928774696171277}, {2031., 0.015928774696171277}, {2032., 0.015928774696171277}, {2033., 0.015928774696171277}, {2034., 0.015928774696171277}, {2035., 0.015928774696171277}, {2036., 0.015928774696171277}, {2037., 0.015928774696171277}, {2038., 0.015928774696171277}, {2039., 0.015928774696171277}, {2040., 0.015928774696171277}}</t>
+    <t>{{2000., 0.13864098572643146}, {2001., 0.14340629366456}, {2002., 0.1533926546653545}, {2003., 0.16104882507175894}, {2004., 0.1668246755307006}, {2005., 0.17346764890542046}, {2006., 0.1747312215393501}, {2007., 0.17317265295543235}, {2008., 0.17724585262134768}, {2009., 0.17721848556437272}, {2010., 0.17935897814424598}, {2011., 0.19300590079202984}, {2012., 0.19975358160153334}, {2013., 0.19346390170954023}, {2014., 0.19052614964266096}, {2015., 0.2015212285097643}, {2016., 0.21341555732729905}, {2017., 0.21874869421670848}, {2018., 0.22417712059578757}, {2019., 0.229700650602687}, {2020., 0.23531899590104544}, {2021., 0.2410317625907375}, {2022., 0.24683844827283563}, {2023., 0.25273843928722356}, {2024., 0.2587310081414289}, {2025., 0.2648153111492287}, {2026., 0.27099038629749445}, {2027., 0.2772551513595062}, {2028., 0.28360840227256345}, {2029., 0.29004881179723346}, {2030., 0.29657492847491906}, {2031., 0.30318517589959865}, {2032., 0.3098778523186577}, {2033., 0.31665113057663824}, {2034., 0.32350305841444466}, {2035., 0.3304315591351837}, {2036., 0.33743443264628276}, {2037., 0.34450935688582884}, {2038., 0.35165388963931127}, {2039., 0.3588654707510448}, {2040., 0.3661414247325031}}</t>
+  </si>
+  <si>
+    <t>{{2000., 0.1768555021487156}, {2001., 0.18383861728486073}, {2002., 0.19852716462262696}, {2003., 0.20990621138828117}, {2004., 0.2185018689228458}, {2005., 0.22839482459544527}, {2006., 0.2302770082363087}, {2007., 0.22795541782866946}, {2008., 0.23402285838768336}, {2009., 0.2339820916357753}, {2010., 0.23717058519084538}, {2011., 0.2574880422390382}, {2012., 0.2675190891056945}, {2013., 0.2581693119640019}, {2014., 0.25379857187026367}, {2015., 0.2701444401142528}, {2016., 0.28777674049828034}, {2017., 0.2956600900752105}, {2018., 0.3036673196694935}, {2019., 0.31179540811423895}, {2020., 0.3200410638604347}, {2021., 0.32840072593067193}, {2022., 0.3368705660427389}, {2023., 0.3454464919375542}, {2024., 0.354124151937876}, {2025., 0.36289894075546947}, {2026., 0.3717660065551432}, {2027., 0.38072025927425535}, {2028., 0.38975638018603576}, {2029., 0.39886883268461476}, {2030., 0.4080518742589872}, {2031., 0.4172995696124214}, {2032., 0.4266058048732826}, {2033., 0.43596430283293636}, {2034., 0.44536863913642843}, {2035., 0.4548122593423193}, {2036., 0.4642884967593518}, {2037., 0.4737905909597184}, {2038., 0.4833117068617834}, {2039., 0.4928449542692211}, {2040., 0.5023834077487089}}</t>
+  </si>
+  <si>
+    <t>{{2000., 0.061012210476429136}, {2001., 0.07611992343485692}, {2002., 0.11720460963536777}, {2003., 0.15837608743771714}, {2004., 0.19429325358995372}, {2005., 0.24008777535914436}, {2006., 0.2473334874696084}, {2007., 0.23292041301835206}, {2008., 0.26133540179634507}, {2009., 0.25830199655178065}, {2010., 0.27187548025831765}, {2011., 0.38388225501367257}, {2012., 0.44236608221165935}, {2013., 0.3858807851434603}, {2014., 0.3599669760232489}, {2015., 0.4583338839300777}, {2016., 0.5637676224864289}, {2017., 0.608440889614856}, {2018., 0.6513683728429689}, {2019., 0.69197218867621}, {2020., 0.7298086363090585}, {2021., 0.7645786663327382}, {2022., 0.7961242142731141}, {2023., 0.8244135126142146}, {2024., 0.8495194144131167}, {2025., 0.8715947077734818}, {2026., 0.8908476808622621}, {2027., 0.907520179270313}, {2028., 0.9218693828470589}, {2029., 0.9341536999768467}, {2030., 0.9446226020095245}, {2031., 0.9535098883606936}, {2032., 0.9610297325083569}, {2033., 0.9673748490784645}, {2034., 0.9727161875475266}, {2035., 0.977203657626819}, {2036., 0.9809674981677456}, {2037., 0.9841200001241508}, {2038., 0.9867573776638039}, {2039., 0.9889616480707373}, {2040., 0.9908024316288423}}</t>
+  </si>
+  <si>
+    <t>{{2000., 0.1102680949505768}, {2001., 0.14164229192572025}, {2002., 0.22679463092517832}, {2003., 0.30875319534428675}, {2004., 0.37591075589588446}, {2005., 0.4548157505898362}, {2006., 0.466591643179902}, {2007., 0.4429766184763935}, {2008., 0.48880160819817575}, {2009., 0.4840508376192788}, {2010., 0.5050491545550977}, {2011., 0.6541930569993194}, {2012., 0.7168178967783682}, {2013., 0.6564918627993113}, {2014., 0.625756997044931}, {2015., 0.732336969060333}, {2016., 0.820115196367716}, {2017., 0.8506013258225014}, {2018., 0.8766975883690794}, {2019., 0.8987779268505394}, {2020., 0.9172773269167419}, {2021., 0.9326491226026863}, {2022., 0.9453347111254137}, {2023., 0.9557443374235848}, {2024., 0.9642466831123514}, {2025., 0.971164850270404}, {2026., 0.9767766119727436}, {2027., 0.9813172488183106}, {2028., 0.9849837485084647}, {2029., 0.9879395390696635}, {2030., 0.9903192317615762}, {2031., 0.9922330702240909}, {2032., 0.9937709324366929}, {2033., 0.9950058285506183}, {2034., 0.995996895949385}, {2035., 0.9967919252735056}, {2036., 0.9974294667264978}, {2037., 0.9979405711818405}, {2038., 0.9983502197689068}, {2039., 0.998678491548566}, {2040., 0.9989415133599091}}</t>
+  </si>
+  <si>
+    <t>{{2000., 0.004220435148378841}, {2001., 0.004845244769950683}, {2002., 0.006392298956836001}, {2003., 0.007825403118496303}, {2004., 0.009700553933431767}, {2005., 0.013233498109421711}, {2006., 0.01577081854989373}, {2007., 0.017517065161890034}, {2008., 0.023145702820823785}, {2009., 0.026951472499235293}, {2010., 0.034332066465764685}, {2011., 0.06425028871343376}, {2012., 0.08702223571306184}, {2013., 0.07117972371357126}, {2014., 0.06461864557199926}, {2015., 0.09194046647068263}, {2016., 0.13081317326553019}, {2017., 0.15170365546154818}, {2018., 0.1752576056882522}, {2019., 0.2015995034981771}, {2020., 0.23079273839492873}, {2021., 0.26282178566099695}, {2022., 0.29757619950368275}, {2023., 0.33483890796005417}, {2024., 0.3742814019899951}, {2025., 0.4154680005451366}, {2026., 0.45787036877414955}, {2027., 0.500891962133672}, {2028., 0.5439003523460016}, {2029., 0.586263884289366}, {2030., 0.6273882382707183}, {2031., 0.6667484915682909}, {2032., 0.703913180705032}, {2033., 0.7385583903868201}, {2034., 0.7704716108967044}, {2035., 0.7995465938929365}, {2036., 0.8257714171384778}, {2037., 0.8492123554312975}, {2038., 0.8699960289057868}, {2039., 0.8882918359910112}, {2040., 0.9042960680403596}}</t>
+  </si>
+  <si>
+    <t>{{2000., 0.006685613708698735}, {2001., 0.00790708866323162}, {2002., 0.011069442730743754}, {2003., 0.014145170149070782}, {2004., 0.018342488929644626}, {2005., 0.026671000077150255}, {2006., 0.032919471065464466}, {2007., 0.037324673385856856}, {2008., 0.051982783065088876}, {2009., 0.062200927531774926}, {2010., 0.08249767349796562}, {2011., 0.16704777860189307}, {2012., 0.23024778554309192}, {2013., 0.18651655917404847}, {2014., 0.16808661534406064}, {2015., 0.24354848654478756}, {2016., 0.3429415200700157}, {2017., 0.3917443380456915}, {2018., 0.4428116961324038}, {2019., 0.49511730260211023}, {2020., 0.5475300057536283}, {2021., 0.5989094104481839}, {2022., 0.6482031488460581}, {2023., 0.6945713926513444}, {2024., 0.7373106225045547}, {2025., 0.7759980291938543}, {2026., 0.8104525257671122}, {2027., 0.8406954071267727}, {2028., 0.8669053745856697}, {2029., 0.8893705467058338}, {2030., 0.908444273026314}, {2031., 0.9245086159933302}, {2032., 0.9379468470663223}, {2033., 0.9491245756769737}, {2034., 0.9583781913069924}, {2035., 0.9660089653729551}, {2036., 0.9722812067706159}, {2037., 0.9774231041952759}, {2038., 0.9816291905254266}, {2039., 0.985063655392439}, {2040., 0.9878639773343165}}</t>
+  </si>
+  <si>
+    <t>{{2014., 0.19052614964266096}, {2015., 0.19256548156677758}, {2016., 0.19256548156677758}, {2017., 0.19256548156677758}, {2018., 0.1875497056708232}, {2019., 0.1778209444730249}, {2020., 0.16849218283877274}, {2021., 0.15955784581352933}, {2022., 0.15101121658004787}, {2023., 0.14284457431397882}, {2024., 0.13890109406273876}, {2025., 0.13890109406273876}, {2026., 0.13890109406273876}, {2027., 0.13890109406273876}, {2028., 0.13890109406273876}, {2029., 0.13890109406273876}, {2030., 0.13890109406273876}, {2031., 0.13890109406273876}, {2032., 0.13890109406273876}, {2033., 0.13890109406273876}, {2034., 0.13890109406273876}, {2035., 0.13890109406273876}, {2036., 0.13890109406273876}, {2037., 0.13890109406273876}, {2038., 0.13890109406273876}, {2039., 0.13890109406273876}, {2040., 0.13890109406273876}}</t>
+  </si>
+  <si>
+    <t>{{2014., 0.25379857187026367}, {2015., 0.256832875486047}, {2016., 0.256832875486047}, {2017., 0.256832875486047}, {2018., 0.24936838133152966}, {2019., 0.23487952964530895}, {2020., 0.22098467757161058}, {2021., 0.20768868451698633}, {2022., 0.19500794406764477}, {2023., 0.18301477418606749}, {2024., 0.17723630471125335}, {2025., 0.17723630471125335}, {2026., 0.17723630471125335}, {2027., 0.17723630471125335}, {2028., 0.17723630471125335}, {2029., 0.17723630471125335}, {2030., 0.17723630471125335}, {2031., 0.17723630471125335}, {2032., 0.17723630471125335}, {2033., 0.17723630471125335}, {2034., 0.17723630471125335}, {2035., 0.17723630471125335}, {2036., 0.17723630471125335}, {2037., 0.17723630471125335}, {2038., 0.17723630471125335}, {2039., 0.17723630471125335}, {2040., 0.17723630471125335}}</t>
+  </si>
+  <si>
+    <t>{{2014., 0.3599669760232489}, {2015., 0.3779114109136408}, {2016., 0.3779114109136408}, {2017., 0.3779114109136408}, {2018., 0.3342210124299232}, {2019., 0.25528511452836544}, {2020., 0.18968080200769777}, {2021., 0.13781582459288702}, {2022., 0.09841014018463021}, {2023., 0.06936523998333025}, {2024., 0.058019053232080474}, {2025., 0.058019053232080474}, {2026., 0.058019053232080474}, {2027., 0.058019053232080474}, {2028., 0.058019053232080474}, {2029., 0.058019053232080474}, {2030., 0.058019053232080474}, {2031., 0.058019053232080474}, {2032., 0.058019053232080474}, {2033., 0.058019053232080474}, {2034., 0.058019053232080474}, {2035., 0.058019053232080474}, {2036., 0.058019053232080474}, {2037., 0.058019053232080474}, {2038., 0.058019053232080474}, {2039., 0.058019053232080474}, {2040., 0.058019053232080474}}</t>
+  </si>
+  <si>
+    <t>{{2014., 0.625756997044931}, {2015., 0.647254825382658}, {2016., 0.647254825382658}, {2017., 0.647254825382658}, {2018., 0.5931583013257863}, {2019., 0.47929263262659405}, {2020., 0.36753858730869626}, {2021., 0.2684099337461131}, {2022., 0.18806709082346051}, {2023., 0.1275793732274077}, {2024., 0.10409877266675104}, {2025., 0.10409877266675104}, {2026., 0.10409877266675104}, {2027., 0.10409877266675104}, {2028., 0.10409877266675104}, {2029., 0.10409877266675104}, {2030., 0.10409877266675104}, {2031., 0.10409877266675104}, {2032., 0.10409877266675104}, {2033., 0.10409877266675104}, {2034., 0.10409877266675104}, {2035., 0.10409877266675104}, {2036., 0.10409877266675104}, {2037., 0.10409877266675104}, {2038., 0.10409877266675104}, {2039., 0.10409877266675104}, {2040., 0.10409877266675104}}</t>
+  </si>
+  <si>
+    <t>{{2014., 0.06461864557199926}, {2015., 0.06911873155252335}, {2016., 0.06911873155252335}, {2017., 0.06911873155252335}, {2018., 0.05847966856427177}, {2019., 0.041652923216596395}, {2020., 0.029516066271041853}, {2021., 0.02083875675038981}, {2022., 0.014673882863328866}, {2023., 0.01031359613319445}, {2024., 0.008642049362490632}, {2025., 0.008642049362490632}, {2026., 0.008642049362490632}, {2027., 0.008642049362490632}, {2028., 0.008642049362490632}, {2029., 0.008642049362490632}, {2030., 0.008642049362490632}, {2031., 0.008642049362490632}, {2032., 0.008642049362490632}, {2033., 0.008642049362490632}, {2034., 0.008642049362490632}, {2035., 0.008642049362490632}, {2036., 0.008642049362490632}, {2037., 0.008642049362490632}, {2038., 0.008642049362490632}, {2039., 0.008642049362490632}, {2040., 0.008642049362490632}}</t>
+  </si>
+  <si>
+    <t>{{2014., 0.16808661534406064}, {2015., 0.1807435354798601}, {2016., 0.1807435354798601}, {2017., 0.1807435354798601}, {2018., 0.1507299625602193}, {2019., 0.10302782796890286}, {2020., 0.06919223480218764}, {2021., 0.045900035905414804}, {2022., 0.030194347060225467}, {2023., 0.01975144740515513}, {2024., 0.01595108743112701}, {2025., 0.01595108743112701}, {2026., 0.01595108743112701}, {2027., 0.01595108743112701}, {2028., 0.01595108743112701}, {2029., 0.01595108743112701}, {2030., 0.01595108743112701}, {2031., 0.01595108743112701}, {2032., 0.01595108743112701}, {2033., 0.01595108743112701}, {2034., 0.01595108743112701}, {2035., 0.01595108743112701}, {2036., 0.01595108743112701}, {2037., 0.01595108743112701}, {2038., 0.01595108743112701}, {2039., 0.01595108743112701}, {2040., 0.01595108743112701}}</t>
   </si>
   <si>
     <t>{2000., 0.15774522301751268}</t>
@@ -796,22 +796,22 @@
     <t>{2040., 0.011902055065637712}</t>
   </si>
   <si>
-    <t>{{2000., 0.13853578631707641}, {2001., 0.14334870031974473}, {2002., 0.15343933769177553}, {2003., 0.16117925782508266}, {2004., 0.1670202902235085}, {2005., 0.17374020273849802}, {2006., 0.17501863662285133}, {2007., 0.1734417474242709}, {2008., 0.17756304988979338}, {2009., 0.17753535724882602}, {2010., 0.17970141043615664}, {2011., 0.19351556568143577}, {2012., 0.20034842357482952}, {2013., 0.1939792989142101}, {2014., 0.1910049071412821}, {2015., 0.20213863177780472}, {2016., 0.21418722433649331}, {2017., 0.21959080139163567}, {2018., 0.2250916524897339}, {2019., 0.2306895689993882}, {2020., 0.2363842349042214}, {2021., 0.24217522357498608}, {2022., 0.24806199470930604}, {2023., 0.25104109806217495}, {2024., 0.2520779145158845}, {2025., 0.2531175659083254}, {2026., 0.2531175659083254}, {2027., 0.2531175659083254}, {2028., 0.2531175659083254}, {2029., 0.2531175659083254}, {2030., 0.2531175659083254}, {2031., 0.2531175659083254}, {2032., 0.2531175659083254}, {2033., 0.2531175659083254}, {2034., 0.2531175659083254}, {2035., 0.2531175659083254}, {2036., 0.2531175659083254}, {2037., 0.2531175659083254}, {2038., 0.2531175659083254}, {2039., 0.2531175659083254}, {2040., 0.2531175659083254}}</t>
-  </si>
-  <si>
-    <t>{{2000., 0.17779003343384756}, {2001., 0.1848369219848541}, {2002., 0.19965519201795298}, {2003., 0.21104186375044948}, {2004., 0.2196410674418312}, {2005., 0.22953585759734904}, {2006., 0.2314181267257109}, {2007., 0.22909641892407562}, {2008., 0.23516390241792803}, {2009., 0.23512313821348926}, {2010., 0.23831131833515012}, {2011., 0.2586215375621919}, {2012., 0.26864583836891837}, {2013., 0.25930241337483295}, {2014., 0.2549340343450744}, {2015., 0.27126909467423665}, {2016., 0.2888839482126477}, {2017., 0.29675767464418734}, {2018., 0.30475403478292823}, {2019., 0.3128700019636655}, {2020., 0.3211022828894477}, {2021., 0.32944731871954214}, {2022., 0.3379012873082604}, {2023., 0.34216785578665304}, {2024., 0.3436508475518495}, {2025., 0.34513689455094}, {2026., 0.34513689455094}, {2027., 0.34513689455094}, {2028., 0.34513689455094}, {2029., 0.34513689455094}, {2030., 0.34513689455094}, {2031., 0.34513689455094}, {2032., 0.34513689455094}, {2033., 0.34513689455094}, {2034., 0.34513689455094}, {2035., 0.34513689455094}, {2036., 0.34513689455094}, {2037., 0.34513689455094}, {2038., 0.34513689455094}, {2039., 0.34513689455094}, {2040., 0.34513689455094}}</t>
-  </si>
-  <si>
-    <t>{{2000., 0.0626042080198429}, {2001., 0.07828185182181285}, {2002., 0.12099826774212379}, {2003., 0.16366198507770507}, {2004., 0.20049854347802348}, {2005., 0.2473145590665686}, {2006., 0.25470643379996355}, {2007., 0.23999846173497844}, {2008., 0.268978845725233}, {2009., 0.26588817556872296}, {2010., 0.27971215798178056}, {2011., 0.3932230520697693}, {2012., 0.45209508286717653}, {2013., 0.3952393306704061}, {2014., 0.36907072171796856}, {2015., 0.46812176495997004}, {2016., 0.5734396625600047}, {2017., 0.6178007346694113}, {2018., 0.6602814776922612}, {2019., 0.6806392980086604}, {2020., 0.6867414898043976}, {2021., 0.6927797125890754}, {2022., 0.6927797125890754}, {2023., 0.6927797125890754}, {2024., 0.6927797125890754}, {2025., 0.6927797125890754}, {2026., 0.6927797125890754}, {2027., 0.6927797125890754}, {2028., 0.6927797125890754}, {2029., 0.6927797125890754}, {2030., 0.6927797125890754}, {2031., 0.6927797125890754}, {2032., 0.6927797125890754}, {2033., 0.6927797125890754}, {2034., 0.6927797125890754}, {2035., 0.6927797125890754}, {2036., 0.6927797125890754}, {2037., 0.6927797125890754}, {2038., 0.6927797125890754}, {2039., 0.6927797125890754}, {2040., 0.6927797125890754}}</t>
-  </si>
-  <si>
-    <t>{{2000., 0.11341260818775203}, {2001., 0.14596871370570527}, {2002., 0.23426866295908763}, {2003., 0.31892802251995606}, {2004., 0.38792268641414973}, {2005., 0.46844681062458376}, {2006., 0.4804086349471679}, {2007., 0.4564055669953613}, {2008., 0.5029272342798269}, {2009., 0.4981151391638927}, {2010., 0.5193648131117024}, {2011., 0.6687211359701506}, {2012., 0.7305533231766058}, {2013., 0.671001375145701}, {2014., 0.6404607203482999}, {2015., 0.7457800707439324}, {2016., 0.8311131594199891}, {2017., 0.8604034764358723}, {2018., 0.8853148961587166}, {2019., 0.8962567012210152}, {2020., 0.8994174557252128}, {2021., 0.9024923880700098}, {2022., 0.9024923880700098}, {2023., 0.9024923880700098}, {2024., 0.9024923880700098}, {2025., 0.9024923880700098}, {2026., 0.9024923880700098}, {2027., 0.9024923880700098}, {2028., 0.9024923880700098}, {2029., 0.9024923880700098}, {2030., 0.9024923880700098}, {2031., 0.9024923880700098}, {2032., 0.9024923880700098}, {2033., 0.9024923880700098}, {2034., 0.9024923880700098}, {2035., 0.9024923880700098}, {2036., 0.9024923880700098}, {2037., 0.9024923880700098}, {2038., 0.9024923880700098}, {2039., 0.9024923880700098}, {2040., 0.9024923880700098}}</t>
-  </si>
-  <si>
-    <t>{{2000., 0.004245667881577086}, {2001., 0.004874671535597712}, {2002., 0.006432322750266142}, {2003., 0.007875456858226432}, {2004., 0.009763968474068623}, {2005., 0.013322623847923817}, {2006., 0.015878728835289017}, {2007., 0.01763802116239439}, {2008., 0.023309190697007875}, {2009., 0.027144017106482086}, {2010., 0.034581371851898364}, {2011., 0.06473052508448475}, {2012., 0.08767532860592818}, {2013., 0.07171296748522162}, {2014., 0.06510170723603599}, {2015., 0.0926303218972931}, {2016., 0.13178452070449528}, {2017., 0.15281867943768995}, {2018., 0.17652749826032493}, {2019., 0.20303306200913526}, {2020., 0.23239527455789497}, {2021., 0.26459401101631946}, {2022., 0.2817249104675058}, {2023., 0.2876329566838136}, {2024., 0.2936142539617634}, {2025., 0.2936142539617634}, {2026., 0.2936142539617634}, {2027., 0.2936142539617634}, {2028., 0.2936142539617634}, {2029., 0.2936142539617634}, {2030., 0.2936142539617634}, {2031., 0.2936142539617634}, {2032., 0.2936142539617634}, {2033., 0.2936142539617634}, {2034., 0.2936142539617634}, {2035., 0.2936142539617634}, {2036., 0.2936142539617634}, {2037., 0.2936142539617634}, {2038., 0.2936142539617634}, {2039., 0.2936142539617634}, {2040., 0.2936142539617634}}</t>
-  </si>
-  <si>
-    <t>{{2000., 0.0066921836593021936}, {2001., 0.007910345154487044}, {2002., 0.011061368771239552}, {2003., 0.014123144211918903}, {2004., 0.018321636382292398}, {2005., 0.026659366655086326}, {2006., 0.03291801690740733}, {2007., 0.03733171127755734}, {2008., 0.05202414690300587}, {2009., 0.06227050526078328}, {2010., 0.08263074785857878}, {2011., 0.1674998458143094}, {2012., 0.23095523189373252}, {2013., 0.18704726231150867}, {2014., 0.16854286173802427}, {2015., 0.2443090418834672}, {2016., 0.3440736651995076}, {2017., 0.39303430700301767}, {2018., 0.44424334921232117}, {2019., 0.4966648793326893}, {2020., 0.5491598351588212}, {2021., 0.6005827937086953}, {2022., 0.625556956316057}, {2023., 0.6338118420192975}, {2024., 0.6419888940140313}, {2025., 0.6419888940140313}, {2026., 0.6419888940140313}, {2027., 0.6419888940140313}, {2028., 0.6419888940140313}, {2029., 0.6419888940140313}, {2030., 0.6419888940140313}, {2031., 0.6419888940140313}, {2032., 0.6419888940140313}, {2033., 0.6419888940140313}, {2034., 0.6419888940140313}, {2035., 0.6419888940140313}, {2036., 0.6419888940140313}, {2037., 0.6419888940140313}, {2038., 0.6419888940140313}, {2039., 0.6419888940140313}, {2040., 0.6419888940140313}}</t>
+    <t>{{2000., 0.13864098572643146}, {2001., 0.14340629366456}, {2002., 0.1533926546653545}, {2003., 0.16104882507175894}, {2004., 0.1668246755307006}, {2005., 0.17346764890542046}, {2006., 0.1747312215393501}, {2007., 0.17317265295543235}, {2008., 0.17724585262134768}, {2009., 0.17721848556437272}, {2010., 0.17935897814424598}, {2011., 0.19300590079202984}, {2012., 0.19975358160153334}, {2013., 0.19346390170954023}, {2014., 0.19052614964266096}, {2015., 0.2015212285097643}, {2016., 0.21341555732729905}, {2017., 0.21874869421670848}, {2018., 0.22417712059578757}, {2019., 0.229700650602687}, {2020., 0.23531899590104544}, {2021., 0.2410317625907375}, {2022., 0.24683844827283563}, {2023., 0.24977682338508525}, {2024., 0.2507994357450421}, {2025., 0.2518248294576295}, {2026., 0.2518248294576295}, {2027., 0.2518248294576295}, {2028., 0.2518248294576295}, {2029., 0.2518248294576295}, {2030., 0.2518248294576295}, {2031., 0.2518248294576295}, {2032., 0.2518248294576295}, {2033., 0.2518248294576295}, {2034., 0.2518248294576295}, {2035., 0.2518248294576295}, {2036., 0.2518248294576295}, {2037., 0.2518248294576295}, {2038., 0.2518248294576295}, {2039., 0.2518248294576295}, {2040., 0.2518248294576295}}</t>
+  </si>
+  <si>
+    <t>{{2000., 0.1768555021487156}, {2001., 0.18383861728486073}, {2002., 0.19852716462262696}, {2003., 0.20990621138828117}, {2004., 0.2185018689228458}, {2005., 0.22839482459544527}, {2006., 0.2302770082363087}, {2007., 0.22795541782866946}, {2008., 0.23402285838768336}, {2009., 0.2339820916357753}, {2010., 0.23717058519084538}, {2011., 0.2574880422390382}, {2012., 0.2675190891056945}, {2013., 0.2581693119640019}, {2014., 0.25379857187026367}, {2015., 0.2701444401142528}, {2016., 0.28777674049828034}, {2017., 0.2956600900752105}, {2018., 0.3036673196694935}, {2019., 0.31179540811423895}, {2020., 0.3200410638604347}, {2021., 0.32840072593067193}, {2022., 0.3368705660427389}, {2023., 0.34114553422894406}, {2024., 0.3426315054270273}, {2025., 0.3441205685940211}, {2026., 0.3441205685940211}, {2027., 0.3441205685940211}, {2028., 0.3441205685940211}, {2029., 0.3441205685940211}, {2030., 0.3441205685940211}, {2031., 0.3441205685940211}, {2032., 0.3441205685940211}, {2033., 0.3441205685940211}, {2034., 0.3441205685940211}, {2035., 0.3441205685940211}, {2036., 0.3441205685940211}, {2037., 0.3441205685940211}, {2038., 0.3441205685940211}, {2039., 0.3441205685940211}, {2040., 0.3441205685940211}}</t>
+  </si>
+  <si>
+    <t>{{2000., 0.061012210476429136}, {2001., 0.07611992343485692}, {2002., 0.11720460963536777}, {2003., 0.15837608743771714}, {2004., 0.19429325358995372}, {2005., 0.24008777535914436}, {2006., 0.2473334874696084}, {2007., 0.23292041301835206}, {2008., 0.26133540179634507}, {2009., 0.25830199655178065}, {2010., 0.27187548025831765}, {2011., 0.38388225501367257}, {2012., 0.44236608221165935}, {2013., 0.3858807851434603}, {2014., 0.3599669760232489}, {2015., 0.4583338839300777}, {2016., 0.5637676224864289}, {2017., 0.608440889614856}, {2018., 0.6513683728429689}, {2019., 0.67199181251241}, {2020., 0.678180150630938}, {2021., 0.684306585524787}, {2022., 0.684306585524787}, {2023., 0.684306585524787}, {2024., 0.684306585524787}, {2025., 0.684306585524787}, {2026., 0.684306585524787}, {2027., 0.684306585524787}, {2028., 0.684306585524787}, {2029., 0.684306585524787}, {2030., 0.684306585524787}, {2031., 0.684306585524787}, {2032., 0.684306585524787}, {2033., 0.684306585524787}, {2034., 0.684306585524787}, {2035., 0.684306585524787}, {2036., 0.684306585524787}, {2037., 0.684306585524787}, {2038., 0.684306585524787}, {2039., 0.684306585524787}, {2040., 0.684306585524787}}</t>
+  </si>
+  <si>
+    <t>{{2000., 0.1102680949505768}, {2001., 0.14164229192572025}, {2002., 0.22679463092517832}, {2003., 0.30875319534428675}, {2004., 0.37591075589588446}, {2005., 0.4548157505898362}, {2006., 0.466591643179902}, {2007., 0.4429766184763935}, {2008., 0.48880160819817575}, {2009., 0.4840508376192788}, {2010., 0.5050491545550977}, {2011., 0.6541930569993194}, {2012., 0.7168178967783682}, {2013., 0.6564918627993113}, {2014., 0.625756997044931}, {2015., 0.732336969060333}, {2016., 0.820115196367716}, {2017., 0.8506013258225014}, {2018., 0.8766975883690794}, {2019., 0.8882134301610412}, {2020., 0.8915465145958934}, {2021., 0.8947919896857224}, {2022., 0.8947919896857224}, {2023., 0.8947919896857224}, {2024., 0.8947919896857224}, {2025., 0.8947919896857224}, {2026., 0.8947919896857224}, {2027., 0.8947919896857224}, {2028., 0.8947919896857224}, {2029., 0.8947919896857224}, {2030., 0.8947919896857224}, {2031., 0.8947919896857224}, {2032., 0.8947919896857224}, {2033., 0.8947919896857224}, {2034., 0.8947919896857224}, {2035., 0.8947919896857224}, {2036., 0.8947919896857224}, {2037., 0.8947919896857224}, {2038., 0.8947919896857224}, {2039., 0.8947919896857224}, {2040., 0.8947919896857224}}</t>
+  </si>
+  <si>
+    <t>{{2000., 0.004220435148378841}, {2001., 0.004845244769950683}, {2002., 0.006392298956836001}, {2003., 0.007825403118496303}, {2004., 0.009700553933431767}, {2005., 0.013233498109421711}, {2006., 0.01577081854989373}, {2007., 0.017517065161890034}, {2008., 0.023145702820823785}, {2009., 0.026951472499235293}, {2010., 0.034332066465764685}, {2011., 0.06425028871343376}, {2012., 0.08702223571306184}, {2013., 0.07117972371357126}, {2014., 0.06461864557199926}, {2015., 0.09194046647068263}, {2016., 0.13081317326553019}, {2017., 0.15170365546154818}, {2018., 0.1752576056882522}, {2019., 0.2015995034981771}, {2020., 0.23079273839492873}, {2021., 0.26282178566099695}, {2022., 0.2798692935847106}, {2023., 0.2857497133459826}, {2024., 0.2917036398156778}, {2025., 0.2917036398156778}, {2026., 0.2917036398156778}, {2027., 0.2917036398156778}, {2028., 0.2917036398156778}, {2029., 0.2917036398156778}, {2030., 0.2917036398156778}, {2031., 0.2917036398156778}, {2032., 0.2917036398156778}, {2033., 0.2917036398156778}, {2034., 0.2917036398156778}, {2035., 0.2917036398156778}, {2036., 0.2917036398156778}, {2037., 0.2917036398156778}, {2038., 0.2917036398156778}, {2039., 0.2917036398156778}, {2040., 0.2917036398156778}}</t>
+  </si>
+  <si>
+    <t>{{2000., 0.006685613708698735}, {2001., 0.00790708866323162}, {2002., 0.011069442730743754}, {2003., 0.014145170149070782}, {2004., 0.018342488929644626}, {2005., 0.026671000077150255}, {2006., 0.032919471065464466}, {2007., 0.037324673385856856}, {2008., 0.051982783065088876}, {2009., 0.062200927531774926}, {2010., 0.08249767349796562}, {2011., 0.16704777860189307}, {2012., 0.23024778554309192}, {2013., 0.18651655917404847}, {2014., 0.16808661534406064}, {2015., 0.24354848654478756}, {2016., 0.3429415200700157}, {2017., 0.3917443380456915}, {2018., 0.4428116961324038}, {2019., 0.49511730260211023}, {2020., 0.5475300057536283}, {2021., 0.5989094104481839}, {2022., 0.623876915063107}, {2023., 0.632131810330542}, {2024., 0.6403099861427145}, {2025., 0.6403099861427145}, {2026., 0.6403099861427145}, {2027., 0.6403099861427145}, {2028., 0.6403099861427145}, {2029., 0.6403099861427145}, {2030., 0.6403099861427145}, {2031., 0.6403099861427145}, {2032., 0.6403099861427145}, {2033., 0.6403099861427145}, {2034., 0.6403099861427145}, {2035., 0.6403099861427145}, {2036., 0.6403099861427145}, {2037., 0.6403099861427145}, {2038., 0.6403099861427145}, {2039., 0.6403099861427145}, {2040., 0.6403099861427145}}</t>
   </si>
   <si>
     <t>{2023., 0.2950167817245382}</t>

</xml_diff>